<commit_message>
Reporte Diario CABA: 2026-02-04
</commit_message>
<xml_diff>
--- a/data/2026/02/CABA_reporte_20260204.xlsx
+++ b/data/2026/02/CABA_reporte_20260204.xlsx
@@ -444,12 +444,12 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>origen</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>link</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>origen</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
@@ -471,7 +471,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Sin publicaciones detectadas</t>
+          <t>Sin aperturas detectadas</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -479,12 +479,12 @@
           <t>No identificado</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>CABA</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
         <v>0</v>
       </c>

</xml_diff>